<commit_message>
Use lor-eor.py to update Mysql table for a particular generator where the EOR is null Update generator_info.xlsx for Herat  GB 980845
</commit_message>
<xml_diff>
--- a/LOR-EOR/generator_info.xlsx
+++ b/LOR-EOR/generator_info.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamfifield/Documents/GitHub/generator_lor_eor_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_UNHCR\CODE\LOR-EOR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02FE7F9F-ACDF-3546-B1AB-559FA078733F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16460" xr2:uid="{EEB780EC-B533-F34B-8E2B-175728310C6F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26083" windowHeight="11438"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>Meter Serial No.</t>
   </si>
@@ -54,9 +53,6 @@
   </si>
   <si>
     <t>KVA Rating</t>
-  </si>
-  <si>
-    <t>009-80845</t>
   </si>
   <si>
     <t>AFGHEROFO01</t>
@@ -161,7 +157,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -506,21 +502,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF94583D-D162-A949-929E-1D56BD72AED6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.3" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -537,211 +533,214 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>980845</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
       </c>
       <c r="G3">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
       </c>
       <c r="G4">
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
       </c>
       <c r="G5">
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
       </c>
       <c r="G6">
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>26</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>27</v>
       </c>
-      <c r="G7" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>32</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>33</v>
-      </c>
-      <c r="F8" t="s">
-        <v>34</v>
       </c>
       <c r="G8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
         <v>35</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" t="s">
-        <v>36</v>
       </c>
       <c r="G9">
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
         <v>37</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" t="s">
-        <v>38</v>
       </c>
       <c r="G10">
         <v>60</v>

</xml_diff>

<commit_message>
Update generator_info.xlsx spreadsheet Always calc LOR, and improve SQL
</commit_message>
<xml_diff>
--- a/LOR-EOR/generator_info.xlsx
+++ b/LOR-EOR/generator_info.xlsx
@@ -70,9 +70,6 @@
     <t>FO Herat (Genset)</t>
   </si>
   <si>
-    <t>009-80E1F</t>
-  </si>
-  <si>
     <t>AFGJALOSO01</t>
   </si>
   <si>
@@ -82,27 +79,15 @@
     <t>SO Jalalabad G66 (Genset)</t>
   </si>
   <si>
-    <t>009-80DCD</t>
-  </si>
-  <si>
     <t>SO Jalalabad G69 (Genset)</t>
   </si>
   <si>
-    <t>009-80E2A</t>
-  </si>
-  <si>
     <t>SO Jalalabad G68 (Genset)</t>
   </si>
   <si>
-    <t>009-80E29</t>
-  </si>
-  <si>
     <t>SO Jalalabad G67 (Genset)</t>
   </si>
   <si>
-    <t>009-80B76</t>
-  </si>
-  <si>
     <t>NGACLBOFO01</t>
   </si>
   <si>
@@ -121,9 +106,6 @@
     <t>60/20</t>
   </si>
   <si>
-    <t>009-80B1E</t>
-  </si>
-  <si>
     <t>SYRALPOSO01</t>
   </si>
   <si>
@@ -139,19 +121,37 @@
     <t>SO Aleppo (100 KVA)</t>
   </si>
   <si>
-    <t>009-80B1C</t>
-  </si>
-  <si>
     <t>SO Aleppo (135 KVA)</t>
   </si>
   <si>
-    <t>009-80B13</t>
-  </si>
-  <si>
     <t>SO Aleppo (60 KVA)</t>
   </si>
   <si>
     <t>Generator Name</t>
+  </si>
+  <si>
+    <t>980E1F</t>
+  </si>
+  <si>
+    <t>980DCD</t>
+  </si>
+  <si>
+    <t>980E2A</t>
+  </si>
+  <si>
+    <t>980E29</t>
+  </si>
+  <si>
+    <t>980B76</t>
+  </si>
+  <si>
+    <t>980B1E</t>
+  </si>
+  <si>
+    <t>980B1C</t>
+  </si>
+  <si>
+    <t>980B13</t>
   </si>
 </sst>
 </file>
@@ -187,8 +187,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,18 +507,19 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.3" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="18.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -533,14 +535,14 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>980845</v>
       </c>
       <c r="B2" t="s">
@@ -563,14 +565,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -579,21 +581,21 @@
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3">
         <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>15</v>
+      <c r="A4" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -602,21 +604,21 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G4">
         <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>17</v>
+      <c r="A5" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -625,21 +627,21 @@
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G5">
         <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>19</v>
+      <c r="A6" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -648,99 +650,99 @@
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G6">
         <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
+      <c r="G7" t="s">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C8" t="s">
         <v>24</v>
       </c>
-      <c r="E7" t="s">
+      <c r="D8" t="s">
         <v>25</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E8" t="s">
         <v>26</v>
       </c>
-      <c r="G7" t="s">
+      <c r="F8" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" t="s">
-        <v>33</v>
       </c>
       <c r="G8">
         <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>34</v>
+      <c r="A9" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G9">
         <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>36</v>
+      <c r="A10" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
         <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" t="s">
-        <v>37</v>
       </c>
       <c r="G10">
         <v>60</v>
@@ -748,5 +750,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Process all devices in generator_info.xls file
</commit_message>
<xml_diff>
--- a/LOR-EOR/generator_info.xlsx
+++ b/LOR-EOR/generator_info.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>Meter Serial No.</t>
   </si>
@@ -70,6 +70,9 @@
     <t>FO Herat (Genset)</t>
   </si>
   <si>
+    <t>009-80E1F</t>
+  </si>
+  <si>
     <t>AFGJALOSO01</t>
   </si>
   <si>
@@ -79,15 +82,27 @@
     <t>SO Jalalabad G66 (Genset)</t>
   </si>
   <si>
+    <t>009-80DCD</t>
+  </si>
+  <si>
     <t>SO Jalalabad G69 (Genset)</t>
   </si>
   <si>
+    <t>009-80E2A</t>
+  </si>
+  <si>
     <t>SO Jalalabad G68 (Genset)</t>
   </si>
   <si>
+    <t>009-80E29</t>
+  </si>
+  <si>
     <t>SO Jalalabad G67 (Genset)</t>
   </si>
   <si>
+    <t>009-80B76</t>
+  </si>
+  <si>
     <t>NGACLBOFO01</t>
   </si>
   <si>
@@ -106,6 +121,9 @@
     <t>60/20</t>
   </si>
   <si>
+    <t>009-80B1E</t>
+  </si>
+  <si>
     <t>SYRALPOSO01</t>
   </si>
   <si>
@@ -121,37 +139,22 @@
     <t>SO Aleppo (100 KVA)</t>
   </si>
   <si>
+    <t>009-80B1C</t>
+  </si>
+  <si>
     <t>SO Aleppo (135 KVA)</t>
   </si>
   <si>
+    <t>009-80B13</t>
+  </si>
+  <si>
     <t>SO Aleppo (60 KVA)</t>
   </si>
   <si>
     <t>Generator Name</t>
   </si>
   <si>
-    <t>980E1F</t>
-  </si>
-  <si>
-    <t>980DCD</t>
-  </si>
-  <si>
-    <t>980E2A</t>
-  </si>
-  <si>
-    <t>980E29</t>
-  </si>
-  <si>
-    <t>980B76</t>
-  </si>
-  <si>
-    <t>980B1E</t>
-  </si>
-  <si>
-    <t>980B1C</t>
-  </si>
-  <si>
-    <t>980B13</t>
+    <t>009-80845</t>
   </si>
 </sst>
 </file>
@@ -187,9 +190,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,19 +509,19 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A3" sqref="A3:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.3" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.88671875" customWidth="1"/>
     <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -535,15 +537,15 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>980845</v>
+      <c r="A2" t="s">
+        <v>39</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -565,14 +567,14 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>31</v>
+      <c r="A3" t="s">
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -581,21 +583,21 @@
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3">
         <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>32</v>
+      <c r="A4" t="s">
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -604,21 +606,21 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G4">
         <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>33</v>
+      <c r="A5" t="s">
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -627,21 +629,21 @@
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G5">
         <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>34</v>
+      <c r="A6" t="s">
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -650,99 +652,99 @@
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G6">
         <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>35</v>
+      <c r="A7" t="s">
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>36</v>
+      <c r="A8" t="s">
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G8">
         <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>37</v>
+      <c r="A9" t="s">
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G9">
         <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>38</v>
+      <c r="A10" t="s">
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="G10">
         <v>60</v>

</xml_diff>

<commit_message>
Clean up, add comments
</commit_message>
<xml_diff>
--- a/LOR-EOR/generator_info.xlsx
+++ b/LOR-EOR/generator_info.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
   <si>
     <t>Meter Serial No.</t>
   </si>
@@ -155,6 +155,15 @@
   </si>
   <si>
     <t>009-80845</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>first good GB data 1699833600</t>
+  </si>
+  <si>
+    <t>2 generators on 1 GB, not handled yet</t>
   </si>
 </sst>
 </file>
@@ -506,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A6"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.3" x14ac:dyDescent="0.3"/>
@@ -518,9 +527,10 @@
     <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,8 +552,11 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -566,7 +579,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -589,7 +602,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -612,7 +625,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -635,7 +648,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -657,8 +670,11 @@
       <c r="G6">
         <v>150</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -680,8 +696,11 @@
       <c r="G7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -704,7 +723,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -727,7 +746,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Update fuel data to 2024-02-11
</commit_message>
<xml_diff>
--- a/LOR-EOR/generator_info.xlsx
+++ b/LOR-EOR/generator_info.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_UNHCR\CODE\LOR-EOR\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF386D0B-E0D3-4663-862F-F94D5FEC026C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26083" windowHeight="11438"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
   <si>
     <t>Meter Serial No.</t>
   </si>
@@ -164,16 +163,55 @@
   </si>
   <si>
     <t>2 generators on 1 GB, not handled yet</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>SO Tripoli G3</t>
+  </si>
+  <si>
+    <t>009-80DD3</t>
+  </si>
+  <si>
+    <t>009-80DD6</t>
+  </si>
+  <si>
+    <t>009-80DDB</t>
+  </si>
+  <si>
+    <t>SO Tripoli G2</t>
+  </si>
+  <si>
+    <t>SO Tripoli G1</t>
+  </si>
+  <si>
+    <t>009-80DD4</t>
+  </si>
+  <si>
+    <t>009-80A9E</t>
+  </si>
+  <si>
+    <t>Lagos</t>
+  </si>
+  <si>
+    <t>2 generators on 1 GB, not handled yet -- other is 16kVa (not currently used)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -199,8 +237,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,11 +555,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.3" x14ac:dyDescent="0.3"/>
@@ -769,6 +810,94 @@
         <v>60</v>
       </c>
     </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15">
+        <v>88</v>
+      </c>
+      <c r="H15" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add E:\_UNHCR\CODE\nanonets-ocr-sample-python to get genset runtime hours from images Only did 72 images for now, 48 had data --- also got number of starts and asset ID for some
</commit_message>
<xml_diff>
--- a/LOR-EOR/generator_info.xlsx
+++ b/LOR-EOR/generator_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_UNHCR\CODE\LOR-EOR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF386D0B-E0D3-4663-862F-F94D5FEC026C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8961B336-D17D-4623-B1C9-A03EE56DB27D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -556,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.3" x14ac:dyDescent="0.3"/>
@@ -898,6 +898,9 @@
         <v>53</v>
       </c>
     </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Taraba to LOR - EOR TODO update retx Bamyan eyedro 15 min data download for Afghan GEEP site
</commit_message>
<xml_diff>
--- a/LOR-EOR/generator_info.xlsx
+++ b/LOR-EOR/generator_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\_UNHCR\CODE\LOR-EOR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8961B336-D17D-4623-B1C9-A03EE56DB27D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B200BE-201E-47DC-B05A-1ECB1CA28971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
   <si>
     <t>Meter Serial No.</t>
   </si>
@@ -196,6 +196,15 @@
   </si>
   <si>
     <t>2 generators on 1 GB, not handled yet -- other is 16kVa (not currently used)</t>
+  </si>
+  <si>
+    <t>SO Takum (Genset)</t>
+  </si>
+  <si>
+    <t>009-80B7A</t>
+  </si>
+  <si>
+    <t>009-80B77</t>
   </si>
 </sst>
 </file>
@@ -556,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.3" x14ac:dyDescent="0.3"/>
@@ -899,7 +908,38 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>